<commit_message>
Code some feature in Admin view
</commit_message>
<xml_diff>
--- a/UserList.xlsx
+++ b/UserList.xlsx
@@ -1,88 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KhanhBang\CNPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\HK7\CongNghe_PhanMem\Thuc_Hanh\Project\Attendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B042DC-AF72-4507-9587-ED6434310105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="1908" yWindow="396" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>FULLNAME</t>
   </si>
   <si>
-    <t>USER ID</t>
-  </si>
-  <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
     <t>EMAIL</t>
   </si>
   <si>
     <t>GENDER</t>
   </si>
   <si>
-    <t>ROLE</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>1002</t>
-  </si>
-  <si>
     <t>Diep Truong Khanh Bang</t>
   </si>
   <si>
-    <t>bang</t>
-  </si>
-  <si>
-    <t>bang@gmail.com</t>
-  </si>
-  <si>
-    <t>Femal</t>
-  </si>
-  <si>
     <t>Tang Duy Hao</t>
   </si>
   <si>
-    <t>hao</t>
-  </si>
-  <si>
-    <t>hao@gmail.com</t>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>MAJOR</t>
+  </si>
+  <si>
+    <t>Mang may tinh va truyen thong du lieu</t>
+  </si>
+  <si>
+    <t>Khoa hoc may tinh</t>
+  </si>
+  <si>
+    <t>52200238</t>
+  </si>
+  <si>
+    <t>52200210</t>
+  </si>
+  <si>
+    <t>52200243</t>
+  </si>
+  <si>
+    <t>Ho Bao Ngan</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Ky thuat phan mem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -90,7 +100,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -122,8 +132,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,101 +410,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" s="2" t="str">
+        <f>A2&amp;"@student.tdtu.edu.vn"</f>
+        <v>52200238@student.tdtu.edu.vn</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C3" s="2" t="str">
+        <f t="shared" ref="C3:C4" si="0">A3&amp;"@student.tdtu.edu.vn"</f>
+        <v>52200210@student.tdtu.edu.vn</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>123456</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52200243@student.tdtu.edu.vn</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
-        <v>123456</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>